<commit_message>
Added more survey collected since previous update
</commit_message>
<xml_diff>
--- a/Data/Survey results data.xlsx
+++ b/Data/Survey results data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niamh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niamh\Desktop\Capstone SBA22224\Capstone_SBA22224\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C934F955-9B03-4A9F-B61A-A42B7911540C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2B07F4-8FD6-4ADC-AF30-F2F54D274249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{AA13BE89-EF53-4491-BFC8-9FED79CA5C1F}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5426" uniqueCount="859">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5692" uniqueCount="899">
   <si>
     <t>original_text</t>
   </si>
@@ -2614,6 +2613,126 @@
   </si>
   <si>
     <t>I reverse imaged searched a selfie and it under visually similar images it is exclusively asian woman my am I white passing narrative is quaking</t>
+  </si>
+  <si>
+    <t>was not aware that Crocs were appropriate business casual attire.😂</t>
+  </si>
+  <si>
+    <t>@Mythical So worried about him. But if you're looking to save him, based on the topography I'd say it's somewhere on the east coast. Perhaps the Carolinas?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @Mythical So worried about him. But if you're looking to save him, based on the topography I'd say it's somewhere on the east coast. Perhaps the Carolinas?</t>
+  </si>
+  <si>
+    <t>It would be nice if my body would let me sleep…😡</t>
+  </si>
+  <si>
+    <t>It would be nice if my body would let me sleep…</t>
+  </si>
+  <si>
+    <t>now that Im working in the commercial talent business, I cant help but wonder how much Jake from State Farm gets paid. I think about it every time I see a SF commercial😁</t>
+  </si>
+  <si>
+    <t>now that Im working in the commercial talent business, I cant help but wonder how much Jake from State Farm gets paid. I think about it every time I see a SF commercial</t>
+  </si>
+  <si>
+    <t>Poor Steve Clifford. Next hire has to be right to get us from A to B. #Magic😃</t>
+  </si>
+  <si>
+    <t>Poor Steve Clifford. Next hire has to be right to get us from A to B. #Magic</t>
+  </si>
+  <si>
+    <t>All the shade i have been hearing about Ben Platt being unbelievable as a teenager in the @DearEvanHansen movie boggles me. Does nobody have any memories of Grease??? Name 1 actor on that film who believably looked high school age!😒</t>
+  </si>
+  <si>
+    <t>All the shade i have been hearing about Ben Platt being unbelievable as a teenager in the @DearEvanHansen movie boggles me. Does nobody have any memories of Grease??? Name 1 actor on that film who believably looked high school age!</t>
+  </si>
+  <si>
+    <t>the manliest thing I can think of is when the men from the World Cup passionately sing their national anthem😃</t>
+  </si>
+  <si>
+    <t>the manliest thing I can think of is when the men from the World Cup passionately sing their national anthem</t>
+  </si>
+  <si>
+    <t>Making the leap from TopShot…officially purchased my @HouseofKibaa membership this morning. Very excited! Thank you @kibaa_hok and team -- very easy process.</t>
+  </si>
+  <si>
+    <t>Also, hopefully and presumably, the Magic front office continuing to do right by players. Give an opportunity - develop - let them go to a better situation. That's the way to do it.</t>
+  </si>
+  <si>
+    <t>If your website still has a google plus share button, forgive me if Im not tripping over myself to take your information as credible or current.😬</t>
+  </si>
+  <si>
+    <t>If your website still has a google plus share button, forgive me if Im not tripping over myself to take your information as credible or current.</t>
+  </si>
+  <si>
+    <t>was not aware that Crocs were appropriate business casual attire. 🙄</t>
+  </si>
+  <si>
+    <t xml:space="preserve">was not aware that Crocs were appropriate business casual attire. </t>
+  </si>
+  <si>
+    <t>@Mythical So worried about him. But if you're looking to save him, based on the topography I'd say it's somewhere on the east coast. Perhaps the Carolinas? 🤞</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @Mythical So worried about him. But if you're looking to save him, based on the topography I'd say it's somewhere on the east coast. Perhaps the Carolinas? </t>
+  </si>
+  <si>
+    <t>It would be nice if my body would let me sleep… 😫😴</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It would be nice if my body would let me sleep… </t>
+  </si>
+  <si>
+    <t>now that Im working in the commercial talent business, I cant help but wonder how much Jake from State Farm gets paid. I think about it every time I see a SF commercial 🤔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">now that Im working in the commercial talent business, I cant help but wonder how much Jake from State Farm gets paid. I think about it every time I see a SF commercial </t>
+  </si>
+  <si>
+    <t>Making the leap from TopShot…officially purchased my @HouseofKibaa membership this morning. Very excited! Thank you @kibaa_hok and team -- very easy process. 🏡🤲</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Making the leap from TopShot…officially purchased my @HouseofKibaa membership this morning. Very excited! Thank you @kibaa_hok and team -- very easy process. </t>
+  </si>
+  <si>
+    <t>it's too bad i forgot how to play my clarinet so close to my recital 🙈</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it's too bad i forgot how to play my clarinet so close to my recital </t>
+  </si>
+  <si>
+    <t>"but clinton's emails! oh. emm. fucking. gee. clinton's god damnd emails. the humanity of it all. https://t.co/cibY5Tn9s6" 🤬</t>
+  </si>
+  <si>
+    <t>going to class! https://t.co/VgCWGl9YTG</t>
+  </si>
+  <si>
+    <t>can some1 do my geometry hw</t>
+  </si>
+  <si>
+    <t>@adorinqdwt @dwtridesgnf Yes the racist is so cool!!! 🙄</t>
+  </si>
+  <si>
+    <t>Putting the toilet paper roll on so that it hangs under instead of over is a crime worthy of the death penalty 🧻😤</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Putting the toilet paper roll on so that it hangs under instead of over is a crime worthy of the death penalty </t>
+  </si>
+  <si>
+    <t>@avsmph But how can we possibly deal with a human experience we haven't first relentlessly quantified??? 👩‍💻</t>
+  </si>
+  <si>
+    <t>Turned 25 today but woke up with $600 from the IRS in my bank account so quarter life crisis has been postponed</t>
+  </si>
+  <si>
+    <t>Only a a President as strong and decisive as @realDonaldTrump would force the FDA to OK a drug even before clinical trial results are in. No need to wait for such silly formalities - people have been taking the drug for years and most are still alive and fine! #OkToTry #Gotrump https://t.co/IdxTJ7kucp 🤬</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only a a President as strong and decisive as @realDonaldTrump would force the FDA to OK a drug even before clinical trial results are in. No need to wait for such silly formalities - people have been taking the drug for years and most are still alive and fine! #OkToTry #Gotrump https://t.co/IdxTJ7kucp </t>
+  </si>
+  <si>
+    <t>@rolandsmartin @nypost Damn! At my wedding we drank enough to make up for the no shows!</t>
   </si>
 </sst>
 </file>
@@ -2998,10 +3117,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3120B6A-9FC1-436A-93DA-AD6EAA672AA0}">
-  <dimension ref="A1:H775"/>
+  <dimension ref="A1:H813"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A761" workbookViewId="0">
-      <selection activeCell="H776" sqref="H776"/>
+    <sheetView tabSelected="1" topLeftCell="A808" workbookViewId="0">
+      <selection activeCell="E815" sqref="E815"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23164,6 +23283,994 @@
         <v>858</v>
       </c>
     </row>
+    <row r="776" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A776">
+        <v>82</v>
+      </c>
+      <c r="B776" t="s">
+        <v>3</v>
+      </c>
+      <c r="C776" t="s">
+        <v>3</v>
+      </c>
+      <c r="D776" t="s">
+        <v>6</v>
+      </c>
+      <c r="E776" t="s">
+        <v>46</v>
+      </c>
+      <c r="F776" t="s">
+        <v>640</v>
+      </c>
+      <c r="G776" t="s">
+        <v>11</v>
+      </c>
+      <c r="H776" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="777" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A777">
+        <v>82</v>
+      </c>
+      <c r="B777" t="s">
+        <v>3</v>
+      </c>
+      <c r="C777" t="s">
+        <v>3</v>
+      </c>
+      <c r="D777" t="s">
+        <v>6</v>
+      </c>
+      <c r="E777" t="s">
+        <v>46</v>
+      </c>
+      <c r="F777" t="s">
+        <v>861</v>
+      </c>
+      <c r="G777" t="s">
+        <v>38</v>
+      </c>
+      <c r="H777" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="778" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A778">
+        <v>82</v>
+      </c>
+      <c r="B778" t="s">
+        <v>3</v>
+      </c>
+      <c r="C778" t="s">
+        <v>3</v>
+      </c>
+      <c r="D778" t="s">
+        <v>6</v>
+      </c>
+      <c r="E778" t="s">
+        <v>46</v>
+      </c>
+      <c r="F778" t="s">
+        <v>863</v>
+      </c>
+      <c r="G778" t="s">
+        <v>11</v>
+      </c>
+      <c r="H778" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="779" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A779">
+        <v>82</v>
+      </c>
+      <c r="B779" t="s">
+        <v>3</v>
+      </c>
+      <c r="C779" t="s">
+        <v>3</v>
+      </c>
+      <c r="D779" t="s">
+        <v>6</v>
+      </c>
+      <c r="E779" t="s">
+        <v>46</v>
+      </c>
+      <c r="F779" t="s">
+        <v>865</v>
+      </c>
+      <c r="G779" t="s">
+        <v>38</v>
+      </c>
+      <c r="H779" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="780" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A780">
+        <v>82</v>
+      </c>
+      <c r="B780" t="s">
+        <v>3</v>
+      </c>
+      <c r="C780" t="s">
+        <v>3</v>
+      </c>
+      <c r="D780" t="s">
+        <v>6</v>
+      </c>
+      <c r="E780" t="s">
+        <v>46</v>
+      </c>
+      <c r="F780" t="s">
+        <v>867</v>
+      </c>
+      <c r="G780" t="s">
+        <v>15</v>
+      </c>
+      <c r="H780" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="781" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A781">
+        <v>82</v>
+      </c>
+      <c r="B781" t="s">
+        <v>3</v>
+      </c>
+      <c r="C781" t="s">
+        <v>3</v>
+      </c>
+      <c r="D781" t="s">
+        <v>6</v>
+      </c>
+      <c r="E781" t="s">
+        <v>46</v>
+      </c>
+      <c r="F781" t="s">
+        <v>869</v>
+      </c>
+      <c r="G781" t="s">
+        <v>11</v>
+      </c>
+      <c r="H781" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="782" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A782">
+        <v>82</v>
+      </c>
+      <c r="B782" t="s">
+        <v>3</v>
+      </c>
+      <c r="C782" t="s">
+        <v>3</v>
+      </c>
+      <c r="D782" t="s">
+        <v>6</v>
+      </c>
+      <c r="E782" t="s">
+        <v>46</v>
+      </c>
+      <c r="F782" t="s">
+        <v>871</v>
+      </c>
+      <c r="G782" t="s">
+        <v>11</v>
+      </c>
+      <c r="H782" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="783" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A783">
+        <v>82</v>
+      </c>
+      <c r="B783" t="s">
+        <v>3</v>
+      </c>
+      <c r="C783" t="s">
+        <v>3</v>
+      </c>
+      <c r="D783" t="s">
+        <v>6</v>
+      </c>
+      <c r="E783" t="s">
+        <v>46</v>
+      </c>
+      <c r="F783" t="s">
+        <v>872</v>
+      </c>
+      <c r="G783" t="s">
+        <v>38</v>
+      </c>
+      <c r="H783" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="784" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A784">
+        <v>82</v>
+      </c>
+      <c r="B784" t="s">
+        <v>3</v>
+      </c>
+      <c r="C784" t="s">
+        <v>3</v>
+      </c>
+      <c r="D784" t="s">
+        <v>6</v>
+      </c>
+      <c r="E784" t="s">
+        <v>46</v>
+      </c>
+      <c r="F784" t="s">
+        <v>873</v>
+      </c>
+      <c r="G784" t="s">
+        <v>11</v>
+      </c>
+      <c r="H784" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="785" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A785">
+        <v>82</v>
+      </c>
+      <c r="B785" t="s">
+        <v>3</v>
+      </c>
+      <c r="C785" t="s">
+        <v>3</v>
+      </c>
+      <c r="D785" t="s">
+        <v>6</v>
+      </c>
+      <c r="E785" t="s">
+        <v>46</v>
+      </c>
+      <c r="F785" t="s">
+        <v>875</v>
+      </c>
+      <c r="G785" t="s">
+        <v>11</v>
+      </c>
+      <c r="H785" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="786" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A786">
+        <v>83</v>
+      </c>
+      <c r="B786" t="s">
+        <v>3</v>
+      </c>
+      <c r="C786" t="s">
+        <v>3</v>
+      </c>
+      <c r="D786" t="s">
+        <v>6</v>
+      </c>
+      <c r="E786" t="s">
+        <v>302</v>
+      </c>
+      <c r="F786" t="s">
+        <v>877</v>
+      </c>
+      <c r="G786" t="s">
+        <v>11</v>
+      </c>
+      <c r="H786" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="787" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A787">
+        <v>83</v>
+      </c>
+      <c r="B787" t="s">
+        <v>3</v>
+      </c>
+      <c r="C787" t="s">
+        <v>3</v>
+      </c>
+      <c r="D787" t="s">
+        <v>6</v>
+      </c>
+      <c r="E787" t="s">
+        <v>302</v>
+      </c>
+      <c r="F787" t="s">
+        <v>879</v>
+      </c>
+      <c r="G787" t="s">
+        <v>38</v>
+      </c>
+      <c r="H787" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="788" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A788">
+        <v>83</v>
+      </c>
+      <c r="B788" t="s">
+        <v>3</v>
+      </c>
+      <c r="C788" t="s">
+        <v>3</v>
+      </c>
+      <c r="D788" t="s">
+        <v>6</v>
+      </c>
+      <c r="E788" t="s">
+        <v>302</v>
+      </c>
+      <c r="F788" t="s">
+        <v>881</v>
+      </c>
+      <c r="G788" t="s">
+        <v>38</v>
+      </c>
+      <c r="H788" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="789" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A789">
+        <v>83</v>
+      </c>
+      <c r="B789" t="s">
+        <v>3</v>
+      </c>
+      <c r="C789" t="s">
+        <v>3</v>
+      </c>
+      <c r="D789" t="s">
+        <v>6</v>
+      </c>
+      <c r="E789" t="s">
+        <v>302</v>
+      </c>
+      <c r="F789" t="s">
+        <v>883</v>
+      </c>
+      <c r="G789" t="s">
+        <v>38</v>
+      </c>
+      <c r="H789" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="790" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A790">
+        <v>83</v>
+      </c>
+      <c r="B790" t="s">
+        <v>3</v>
+      </c>
+      <c r="C790" t="s">
+        <v>3</v>
+      </c>
+      <c r="D790" t="s">
+        <v>6</v>
+      </c>
+      <c r="E790" t="s">
+        <v>302</v>
+      </c>
+      <c r="F790" t="s">
+        <v>867</v>
+      </c>
+      <c r="G790" t="s">
+        <v>15</v>
+      </c>
+      <c r="H790" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="791" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A791">
+        <v>83</v>
+      </c>
+      <c r="B791" t="s">
+        <v>3</v>
+      </c>
+      <c r="C791" t="s">
+        <v>3</v>
+      </c>
+      <c r="D791" t="s">
+        <v>6</v>
+      </c>
+      <c r="E791" t="s">
+        <v>302</v>
+      </c>
+      <c r="F791" t="s">
+        <v>869</v>
+      </c>
+      <c r="G791" t="s">
+        <v>38</v>
+      </c>
+      <c r="H791" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="792" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A792">
+        <v>83</v>
+      </c>
+      <c r="B792" t="s">
+        <v>3</v>
+      </c>
+      <c r="C792" t="s">
+        <v>3</v>
+      </c>
+      <c r="D792" t="s">
+        <v>6</v>
+      </c>
+      <c r="E792" t="s">
+        <v>302</v>
+      </c>
+      <c r="F792" t="s">
+        <v>871</v>
+      </c>
+      <c r="G792" t="s">
+        <v>15</v>
+      </c>
+      <c r="H792" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="793" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A793">
+        <v>83</v>
+      </c>
+      <c r="B793" t="s">
+        <v>3</v>
+      </c>
+      <c r="C793" t="s">
+        <v>3</v>
+      </c>
+      <c r="D793" t="s">
+        <v>6</v>
+      </c>
+      <c r="E793" t="s">
+        <v>302</v>
+      </c>
+      <c r="F793" t="s">
+        <v>885</v>
+      </c>
+      <c r="G793" t="s">
+        <v>38</v>
+      </c>
+      <c r="H793" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="794" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A794">
+        <v>83</v>
+      </c>
+      <c r="B794" t="s">
+        <v>3</v>
+      </c>
+      <c r="C794" t="s">
+        <v>3</v>
+      </c>
+      <c r="D794" t="s">
+        <v>6</v>
+      </c>
+      <c r="E794" t="s">
+        <v>302</v>
+      </c>
+      <c r="F794" t="s">
+        <v>873</v>
+      </c>
+      <c r="G794" t="s">
+        <v>38</v>
+      </c>
+      <c r="H794" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="795" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A795">
+        <v>83</v>
+      </c>
+      <c r="B795" t="s">
+        <v>3</v>
+      </c>
+      <c r="C795" t="s">
+        <v>3</v>
+      </c>
+      <c r="D795" t="s">
+        <v>6</v>
+      </c>
+      <c r="E795" t="s">
+        <v>302</v>
+      </c>
+      <c r="F795" t="s">
+        <v>875</v>
+      </c>
+      <c r="G795" t="s">
+        <v>11</v>
+      </c>
+      <c r="H795" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="796" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A796">
+        <v>84</v>
+      </c>
+      <c r="B796" t="s">
+        <v>3</v>
+      </c>
+      <c r="C796" t="s">
+        <v>3</v>
+      </c>
+      <c r="D796" t="s">
+        <v>32</v>
+      </c>
+      <c r="E796" t="s">
+        <v>302</v>
+      </c>
+      <c r="F796" t="s">
+        <v>887</v>
+      </c>
+      <c r="G796" t="s">
+        <v>11</v>
+      </c>
+      <c r="H796" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="797" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A797">
+        <v>84</v>
+      </c>
+      <c r="B797" t="s">
+        <v>3</v>
+      </c>
+      <c r="C797" t="s">
+        <v>3</v>
+      </c>
+      <c r="D797" t="s">
+        <v>32</v>
+      </c>
+      <c r="E797" t="s">
+        <v>302</v>
+      </c>
+      <c r="F797" t="s">
+        <v>830</v>
+      </c>
+      <c r="G797" t="s">
+        <v>11</v>
+      </c>
+      <c r="H797" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="798" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A798">
+        <v>84</v>
+      </c>
+      <c r="B798" t="s">
+        <v>3</v>
+      </c>
+      <c r="C798" t="s">
+        <v>3</v>
+      </c>
+      <c r="D798" t="s">
+        <v>32</v>
+      </c>
+      <c r="E798" t="s">
+        <v>302</v>
+      </c>
+      <c r="F798" t="s">
+        <v>889</v>
+      </c>
+      <c r="G798" t="s">
+        <v>15</v>
+      </c>
+      <c r="H798" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="799" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A799">
+        <v>84</v>
+      </c>
+      <c r="B799" t="s">
+        <v>3</v>
+      </c>
+      <c r="C799" t="s">
+        <v>3</v>
+      </c>
+      <c r="D799" t="s">
+        <v>32</v>
+      </c>
+      <c r="E799" t="s">
+        <v>302</v>
+      </c>
+      <c r="F799" t="s">
+        <v>890</v>
+      </c>
+      <c r="G799" t="s">
+        <v>38</v>
+      </c>
+      <c r="H799" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="800" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A800">
+        <v>84</v>
+      </c>
+      <c r="B800" t="s">
+        <v>3</v>
+      </c>
+      <c r="C800" t="s">
+        <v>3</v>
+      </c>
+      <c r="D800" t="s">
+        <v>32</v>
+      </c>
+      <c r="E800" t="s">
+        <v>302</v>
+      </c>
+      <c r="F800" t="s">
+        <v>836</v>
+      </c>
+      <c r="G800" t="s">
+        <v>11</v>
+      </c>
+      <c r="H800" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="801" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A801">
+        <v>84</v>
+      </c>
+      <c r="B801" t="s">
+        <v>3</v>
+      </c>
+      <c r="C801" t="s">
+        <v>3</v>
+      </c>
+      <c r="D801" t="s">
+        <v>32</v>
+      </c>
+      <c r="E801" t="s">
+        <v>302</v>
+      </c>
+      <c r="F801" t="s">
+        <v>893</v>
+      </c>
+      <c r="G801" t="s">
+        <v>11</v>
+      </c>
+      <c r="H801" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="802" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A802">
+        <v>84</v>
+      </c>
+      <c r="B802" t="s">
+        <v>3</v>
+      </c>
+      <c r="C802" t="s">
+        <v>3</v>
+      </c>
+      <c r="D802" t="s">
+        <v>32</v>
+      </c>
+      <c r="E802" t="s">
+        <v>302</v>
+      </c>
+      <c r="F802" t="s">
+        <v>840</v>
+      </c>
+      <c r="G802" t="s">
+        <v>38</v>
+      </c>
+      <c r="H802" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="803" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A803">
+        <v>84</v>
+      </c>
+      <c r="B803" t="s">
+        <v>3</v>
+      </c>
+      <c r="C803" t="s">
+        <v>3</v>
+      </c>
+      <c r="D803" t="s">
+        <v>32</v>
+      </c>
+      <c r="E803" t="s">
+        <v>302</v>
+      </c>
+      <c r="F803" t="s">
+        <v>842</v>
+      </c>
+      <c r="G803" t="s">
+        <v>38</v>
+      </c>
+      <c r="H803" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="804" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A804">
+        <v>84</v>
+      </c>
+      <c r="B804" t="s">
+        <v>3</v>
+      </c>
+      <c r="C804" t="s">
+        <v>3</v>
+      </c>
+      <c r="D804" t="s">
+        <v>32</v>
+      </c>
+      <c r="E804" t="s">
+        <v>302</v>
+      </c>
+      <c r="F804" t="s">
+        <v>844</v>
+      </c>
+      <c r="G804" t="s">
+        <v>38</v>
+      </c>
+      <c r="H804" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="805" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A805">
+        <v>84</v>
+      </c>
+      <c r="B805" t="s">
+        <v>3</v>
+      </c>
+      <c r="C805" t="s">
+        <v>3</v>
+      </c>
+      <c r="D805" t="s">
+        <v>32</v>
+      </c>
+      <c r="E805" t="s">
+        <v>302</v>
+      </c>
+      <c r="F805" t="s">
+        <v>847</v>
+      </c>
+      <c r="G805" t="s">
+        <v>11</v>
+      </c>
+      <c r="H805" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="806" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A806">
+        <v>85</v>
+      </c>
+      <c r="B806" t="s">
+        <v>3</v>
+      </c>
+      <c r="C806" t="s">
+        <v>3</v>
+      </c>
+      <c r="D806" t="s">
+        <v>32</v>
+      </c>
+      <c r="E806" t="s">
+        <v>100</v>
+      </c>
+      <c r="F806" t="s">
+        <v>849</v>
+      </c>
+      <c r="G806" t="s">
+        <v>38</v>
+      </c>
+      <c r="H806" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="807" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A807">
+        <v>85</v>
+      </c>
+      <c r="B807" t="s">
+        <v>3</v>
+      </c>
+      <c r="C807" t="s">
+        <v>3</v>
+      </c>
+      <c r="D807" t="s">
+        <v>32</v>
+      </c>
+      <c r="E807" t="s">
+        <v>100</v>
+      </c>
+      <c r="F807" t="s">
+        <v>850</v>
+      </c>
+      <c r="G807" t="s">
+        <v>38</v>
+      </c>
+      <c r="H807" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="808" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A808">
+        <v>85</v>
+      </c>
+      <c r="B808" t="s">
+        <v>3</v>
+      </c>
+      <c r="C808" t="s">
+        <v>3</v>
+      </c>
+      <c r="D808" t="s">
+        <v>32</v>
+      </c>
+      <c r="E808" t="s">
+        <v>100</v>
+      </c>
+      <c r="F808" t="s">
+        <v>851</v>
+      </c>
+      <c r="G808" t="s">
+        <v>38</v>
+      </c>
+      <c r="H808" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="809" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A809">
+        <v>85</v>
+      </c>
+      <c r="B809" t="s">
+        <v>3</v>
+      </c>
+      <c r="C809" t="s">
+        <v>3</v>
+      </c>
+      <c r="D809" t="s">
+        <v>32</v>
+      </c>
+      <c r="E809" t="s">
+        <v>100</v>
+      </c>
+      <c r="F809" t="s">
+        <v>895</v>
+      </c>
+      <c r="G809" t="s">
+        <v>38</v>
+      </c>
+      <c r="H809" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="810" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A810">
+        <v>85</v>
+      </c>
+      <c r="B810" t="s">
+        <v>3</v>
+      </c>
+      <c r="C810" t="s">
+        <v>3</v>
+      </c>
+      <c r="D810" t="s">
+        <v>32</v>
+      </c>
+      <c r="E810" t="s">
+        <v>100</v>
+      </c>
+      <c r="F810" t="s">
+        <v>897</v>
+      </c>
+      <c r="G810" t="s">
+        <v>11</v>
+      </c>
+      <c r="H810" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="811" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A811">
+        <v>85</v>
+      </c>
+      <c r="B811" t="s">
+        <v>3</v>
+      </c>
+      <c r="C811" t="s">
+        <v>3</v>
+      </c>
+      <c r="D811" t="s">
+        <v>32</v>
+      </c>
+      <c r="E811" t="s">
+        <v>100</v>
+      </c>
+      <c r="F811" t="s">
+        <v>855</v>
+      </c>
+      <c r="G811" t="s">
+        <v>38</v>
+      </c>
+      <c r="H811" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="812" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A812">
+        <v>85</v>
+      </c>
+      <c r="B812" t="s">
+        <v>3</v>
+      </c>
+      <c r="C812" t="s">
+        <v>3</v>
+      </c>
+      <c r="D812" t="s">
+        <v>32</v>
+      </c>
+      <c r="E812" t="s">
+        <v>100</v>
+      </c>
+      <c r="F812" t="s">
+        <v>898</v>
+      </c>
+      <c r="G812" t="s">
+        <v>38</v>
+      </c>
+      <c r="H812" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="813" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A813">
+        <v>85</v>
+      </c>
+      <c r="B813" t="s">
+        <v>3</v>
+      </c>
+      <c r="C813" t="s">
+        <v>3</v>
+      </c>
+      <c r="D813" t="s">
+        <v>32</v>
+      </c>
+      <c r="E813" t="s">
+        <v>100</v>
+      </c>
+      <c r="F813" t="s">
+        <v>858</v>
+      </c>
+      <c r="G813" t="s">
+        <v>38</v>
+      </c>
+      <c r="H813" t="s">
+        <v>858</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>